<commit_message>
Create new node "CreateVariableSQL"
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-configuration/90_VisualModeling_Page/CreateVariableSQL/200_LibFormula_CreateVariable.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-configuration/90_VisualModeling_Page/CreateVariableSQL/200_LibFormula_CreateVariable.xlsx
@@ -106,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="34">
   <si>
     <t>Action</t>
   </si>
@@ -162,18 +162,12 @@
     <t>PageRouters</t>
   </si>
   <si>
-    <t>executeRcode</t>
-  </si>
-  <si>
     <t>String, String, String</t>
   </si>
   <si>
     <t>variablesTable_onClick</t>
   </si>
   <si>
-    <t>writeButton_onClick</t>
-  </si>
-  <si>
     <t>runActionLink_onClick</t>
   </si>
   <si>
@@ -195,9 +189,6 @@
     <t>validate</t>
   </si>
   <si>
-    <t>validateRCode</t>
-  </si>
-  <si>
     <t>searchBox_onSearch</t>
   </si>
   <si>
@@ -211,6 +202,12 @@
   </si>
   <si>
     <t>CreateVariableSQL_PageLib</t>
+  </si>
+  <si>
+    <t>createVariableSQL</t>
+  </si>
+  <si>
+    <t>executeSQLcode</t>
   </si>
 </sst>
 </file>
@@ -832,7 +829,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -840,7 +837,7 @@
         <v>14</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -853,10 +850,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.3"/>
@@ -901,7 +898,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>15</v>
@@ -918,7 +915,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>15</v>
@@ -935,7 +932,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>15</v>
@@ -952,7 +949,7 @@
         <v>17</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>15</v>
@@ -966,10 +963,10 @@
         <v>14</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>18</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>15</v>
@@ -983,16 +980,16 @@
         <v>14</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -1000,16 +997,16 @@
         <v>14</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
@@ -1017,16 +1014,16 @@
         <v>14</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
@@ -1034,7 +1031,7 @@
         <v>14</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>23</v>
@@ -1043,7 +1040,7 @@
         <v>15</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
@@ -1051,16 +1048,16 @@
         <v>14</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
@@ -1068,16 +1065,16 @@
         <v>14</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
@@ -1085,16 +1082,16 @@
         <v>14</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="E13" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
@@ -1102,16 +1099,16 @@
         <v>14</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E14" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
@@ -1119,16 +1116,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E15" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
@@ -1136,50 +1133,16 @@
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" s="5" t="s">
         <v>15</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>